<commit_message>
pequenas mods nos notebooks da unidade 4
</commit_message>
<xml_diff>
--- a/Notebooks/Unidade 4/resultados_gridsearchCV.xlsx
+++ b/Notebooks/Unidade 4/resultados_gridsearchCV.xlsx
@@ -560,16 +560,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.06468830108642579</v>
+        <v>0.07633962631225585</v>
       </c>
       <c r="C2" t="n">
-        <v>0.003954319199629588</v>
+        <v>0.02074279764011377</v>
       </c>
       <c r="D2" t="n">
-        <v>0.2592904090881348</v>
+        <v>0.2543339729309082</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0292295017665244</v>
+        <v>0.01035063928488965</v>
       </c>
       <c r="F2" t="n">
         <v>3</v>
@@ -641,16 +641,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.06047220230102539</v>
+        <v>0.06673617362976074</v>
       </c>
       <c r="C3" t="n">
-        <v>0.002900309634333446</v>
+        <v>0.002448247433804212</v>
       </c>
       <c r="D3" t="n">
-        <v>0.2569715976715088</v>
+        <v>0.294121265411377</v>
       </c>
       <c r="E3" t="n">
-        <v>0.02836556241686191</v>
+        <v>0.0691875972842113</v>
       </c>
       <c r="F3" t="n">
         <v>3</v>
@@ -722,16 +722,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.06128897666931152</v>
+        <v>0.06385512351989746</v>
       </c>
       <c r="C4" t="n">
-        <v>0.001062526328563581</v>
+        <v>0.001170061260147135</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1934468269348145</v>
+        <v>0.2036287784576416</v>
       </c>
       <c r="E4" t="n">
-        <v>0.007314871146791834</v>
+        <v>0.008945215755263723</v>
       </c>
       <c r="F4" t="n">
         <v>3</v>
@@ -803,16 +803,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.05960612297058106</v>
+        <v>0.07987580299377442</v>
       </c>
       <c r="C5" t="n">
-        <v>0.001352354142788606</v>
+        <v>0.0184100325933261</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1874385356903076</v>
+        <v>0.234155797958374</v>
       </c>
       <c r="E5" t="n">
-        <v>0.004760949696930445</v>
+        <v>0.025029728461905</v>
       </c>
       <c r="F5" t="n">
         <v>3</v>
@@ -884,16 +884,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.06073970794677734</v>
+        <v>0.08663024902343749</v>
       </c>
       <c r="C6" t="n">
-        <v>0.002865628125975763</v>
+        <v>0.02480285007467933</v>
       </c>
       <c r="D6" t="n">
-        <v>0.2756172180175781</v>
+        <v>0.4677600860595703</v>
       </c>
       <c r="E6" t="n">
-        <v>0.00550995860170546</v>
+        <v>0.1185483050510801</v>
       </c>
       <c r="F6" t="n">
         <v>5</v>
@@ -965,16 +965,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.05929341316223145</v>
+        <v>0.09374814033508301</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0009671554746471853</v>
+        <v>0.01646580248803083</v>
       </c>
       <c r="D7" t="n">
-        <v>0.284058666229248</v>
+        <v>0.4695443153381348</v>
       </c>
       <c r="E7" t="n">
-        <v>0.02235282700541413</v>
+        <v>0.0853797996697889</v>
       </c>
       <c r="F7" t="n">
         <v>5</v>
@@ -1046,16 +1046,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>0.05868229866027832</v>
+        <v>0.07477412223815919</v>
       </c>
       <c r="C8" t="n">
-        <v>0.00123814578817672</v>
+        <v>0.01018735420539713</v>
       </c>
       <c r="D8" t="n">
-        <v>0.2254419326782227</v>
+        <v>0.3012666702270508</v>
       </c>
       <c r="E8" t="n">
-        <v>0.01042051956417242</v>
+        <v>0.05821066291779752</v>
       </c>
       <c r="F8" t="n">
         <v>5</v>
@@ -1127,16 +1127,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0.06057858467102051</v>
+        <v>0.07215652465820313</v>
       </c>
       <c r="C9" t="n">
-        <v>0.001354508847145547</v>
+        <v>0.008530893259487735</v>
       </c>
       <c r="D9" t="n">
-        <v>0.2198076248168945</v>
+        <v>0.2534438610076905</v>
       </c>
       <c r="E9" t="n">
-        <v>0.006886339035904006</v>
+        <v>0.01644369689215851</v>
       </c>
       <c r="F9" t="n">
         <v>5</v>

</xml_diff>

<commit_message>
adicionado o notebook sobre clusterização da unidade 05
</commit_message>
<xml_diff>
--- a/Notebooks/Unidade 4/resultados_gridsearchCV.xlsx
+++ b/Notebooks/Unidade 4/resultados_gridsearchCV.xlsx
@@ -560,16 +560,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.07633962631225585</v>
+        <v>0.09214415550231933</v>
       </c>
       <c r="C2" t="n">
-        <v>0.02074279764011377</v>
+        <v>0.01068712843943281</v>
       </c>
       <c r="D2" t="n">
-        <v>0.2543339729309082</v>
+        <v>0.5620160579681397</v>
       </c>
       <c r="E2" t="n">
-        <v>0.01035063928488965</v>
+        <v>0.1879694053081425</v>
       </c>
       <c r="F2" t="n">
         <v>3</v>
@@ -641,16 +641,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.06673617362976074</v>
+        <v>0.08284244537353516</v>
       </c>
       <c r="C3" t="n">
-        <v>0.002448247433804212</v>
+        <v>0.003576248863731651</v>
       </c>
       <c r="D3" t="n">
-        <v>0.294121265411377</v>
+        <v>0.4092443466186523</v>
       </c>
       <c r="E3" t="n">
-        <v>0.0691875972842113</v>
+        <v>0.02078270958990371</v>
       </c>
       <c r="F3" t="n">
         <v>3</v>
@@ -722,16 +722,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.06385512351989746</v>
+        <v>0.08499932289123535</v>
       </c>
       <c r="C4" t="n">
-        <v>0.001170061260147135</v>
+        <v>0.002901952515569321</v>
       </c>
       <c r="D4" t="n">
-        <v>0.2036287784576416</v>
+        <v>0.3371630191802978</v>
       </c>
       <c r="E4" t="n">
-        <v>0.008945215755263723</v>
+        <v>0.03410400802716913</v>
       </c>
       <c r="F4" t="n">
         <v>3</v>
@@ -803,16 +803,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.07987580299377442</v>
+        <v>0.0894345760345459</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0184100325933261</v>
+        <v>0.004878562157682315</v>
       </c>
       <c r="D5" t="n">
-        <v>0.234155797958374</v>
+        <v>0.3135540962219238</v>
       </c>
       <c r="E5" t="n">
-        <v>0.025029728461905</v>
+        <v>0.02533646317474679</v>
       </c>
       <c r="F5" t="n">
         <v>3</v>
@@ -884,16 +884,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.08663024902343749</v>
+        <v>0.08511719703674317</v>
       </c>
       <c r="C6" t="n">
-        <v>0.02480285007467933</v>
+        <v>0.004477371024013886</v>
       </c>
       <c r="D6" t="n">
-        <v>0.4677600860595703</v>
+        <v>0.4835751533508301</v>
       </c>
       <c r="E6" t="n">
-        <v>0.1185483050510801</v>
+        <v>0.02100817168785565</v>
       </c>
       <c r="F6" t="n">
         <v>5</v>
@@ -965,16 +965,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.09374814033508301</v>
+        <v>0.1023220539093018</v>
       </c>
       <c r="C7" t="n">
-        <v>0.01646580248803083</v>
+        <v>0.01750774223661531</v>
       </c>
       <c r="D7" t="n">
-        <v>0.4695443153381348</v>
+        <v>0.5892225742340088</v>
       </c>
       <c r="E7" t="n">
-        <v>0.0853797996697889</v>
+        <v>0.1146882500822285</v>
       </c>
       <c r="F7" t="n">
         <v>5</v>
@@ -1046,16 +1046,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>0.07477412223815919</v>
+        <v>0.08663473129272461</v>
       </c>
       <c r="C8" t="n">
-        <v>0.01018735420539713</v>
+        <v>0.0050290070404196</v>
       </c>
       <c r="D8" t="n">
-        <v>0.3012666702270508</v>
+        <v>0.3810472011566162</v>
       </c>
       <c r="E8" t="n">
-        <v>0.05821066291779752</v>
+        <v>0.02514631095327748</v>
       </c>
       <c r="F8" t="n">
         <v>5</v>
@@ -1127,16 +1127,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0.07215652465820313</v>
+        <v>0.08413500785827636</v>
       </c>
       <c r="C9" t="n">
-        <v>0.008530893259487735</v>
+        <v>0.004418511037569464</v>
       </c>
       <c r="D9" t="n">
-        <v>0.2534438610076905</v>
+        <v>0.344151496887207</v>
       </c>
       <c r="E9" t="n">
-        <v>0.01644369689215851</v>
+        <v>0.01693298457819821</v>
       </c>
       <c r="F9" t="n">
         <v>5</v>

</xml_diff>